<commit_message>
Updated covid_status_usa with latest numbers and fixed line returns in readme
</commit_message>
<xml_diff>
--- a/covid_stats_usa.xlsx
+++ b/covid_stats_usa.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPatel\Documents\code-repos\personal_projects\covid-19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D8637BE7-56E0-4FB6-B694-5AEF190E940F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1260BC33-5C79-4308-AE0A-1CFC34117E63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4777" yWindow="2258" windowWidth="16875" windowHeight="10522" xr2:uid="{FB52F31D-0F16-4780-8438-F4ABCDF0A9C9}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{FB52F31D-0F16-4780-8438-F4ABCDF0A9C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -397,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D6A934D-D9C4-4019-B15A-95629D41A30E}">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -499,7 +499,7 @@
         <v>319</v>
       </c>
       <c r="C7">
-        <f t="shared" ref="C7:C27" si="2">B7-B6</f>
+        <f t="shared" ref="C7:C29" si="2">B7-B6</f>
         <v>98</v>
       </c>
       <c r="D7">
@@ -519,7 +519,7 @@
         <v>116</v>
       </c>
       <c r="D8">
-        <f t="shared" ref="D8:D27" si="3">C8/C7</f>
+        <f t="shared" ref="D8:D29" si="3">C8/C7</f>
         <v>1.1836734693877551</v>
       </c>
     </row>
@@ -816,15 +816,47 @@
         <v>43916</v>
       </c>
       <c r="B27">
-        <v>85377</v>
+        <v>85435</v>
       </c>
       <c r="C27">
         <f t="shared" si="2"/>
-        <v>17166</v>
+        <v>17224</v>
       </c>
       <c r="D27">
         <f t="shared" si="3"/>
-        <v>1.285361287907151</v>
+        <v>1.289704230625234</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A28" s="1">
+        <v>43917</v>
+      </c>
+      <c r="B28">
+        <v>104126</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="2"/>
+        <v>18691</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="3"/>
+        <v>1.0851718532280539</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A29" s="1">
+        <v>43918</v>
+      </c>
+      <c r="B29">
+        <v>123578</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="2"/>
+        <v>19452</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="3"/>
+        <v>1.0407147825156493</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added SIR model sample code, updated COVID-19 stats, and changed the application of drift
</commit_message>
<xml_diff>
--- a/covid_stats_usa.xlsx
+++ b/covid_stats_usa.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPatel\Documents\code-repos\personal_projects\covid-19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1260BC33-5C79-4308-AE0A-1CFC34117E63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0456ACF-6CC4-4963-8789-DE07FFD9F2DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{FB52F31D-0F16-4780-8438-F4ABCDF0A9C9}"/>
+    <workbookView xWindow="4095" yWindow="1927" windowWidth="16875" windowHeight="10531" xr2:uid="{FB52F31D-0F16-4780-8438-F4ABCDF0A9C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -397,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D6A934D-D9C4-4019-B15A-95629D41A30E}">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -499,7 +499,7 @@
         <v>319</v>
       </c>
       <c r="C7">
-        <f t="shared" ref="C7:C29" si="2">B7-B6</f>
+        <f t="shared" ref="C7:C34" si="2">B7-B6</f>
         <v>98</v>
       </c>
       <c r="D7">
@@ -519,7 +519,7 @@
         <v>116</v>
       </c>
       <c r="D8">
-        <f t="shared" ref="D8:D29" si="3">C8/C7</f>
+        <f t="shared" ref="D8:D34" si="3">C8/C7</f>
         <v>1.1836734693877551</v>
       </c>
     </row>
@@ -857,6 +857,86 @@
       <c r="D29">
         <f t="shared" si="3"/>
         <v>1.0407147825156493</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A30" s="1">
+        <v>43919</v>
+      </c>
+      <c r="B30">
+        <v>143491</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="2"/>
+        <v>19913</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="3"/>
+        <v>1.0236993625334156</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A31" s="1">
+        <v>43920</v>
+      </c>
+      <c r="B31">
+        <v>163788</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="2"/>
+        <v>20297</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="3"/>
+        <v>1.019283884899312</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A32" s="1">
+        <v>43921</v>
+      </c>
+      <c r="B32">
+        <v>188530</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="2"/>
+        <v>24742</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="3"/>
+        <v>1.2189978814603144</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A33" s="1">
+        <v>43922</v>
+      </c>
+      <c r="B33">
+        <v>215003</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="2"/>
+        <v>26473</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="3"/>
+        <v>1.0699620079217524</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A34" s="1">
+        <v>43923</v>
+      </c>
+      <c r="B34">
+        <v>244877</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="2"/>
+        <v>29874</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="3"/>
+        <v>1.1284705171306615</v>
       </c>
     </row>
   </sheetData>

</xml_diff>